<commit_message>
DD_KARMEN_TRACY: removed duplicate Alter_BE
</commit_message>
<xml_diff>
--- a/Tracy/DD_KARMEN_TRACY.xlsx
+++ b/Tracy/DD_KARMEN_TRACY.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Tracy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5BB594-4559-484E-B846-3DDDE69AA4AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4690A213-85B2-4516-A8E7-DC9754B9DBF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11340" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>index</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>postmenopausal</t>
-  </si>
-  <si>
-    <t>Age at end of follow-up</t>
   </si>
 </sst>
 </file>
@@ -156,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,9 +186,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,7 +504,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,15 +594,9 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7"/>
-      <c r="B7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8"/>
@@ -1128,9 +1116,6 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1224,18 +1209,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -1476,6 +1449,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -1485,23 +1470,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607F74A7-32EE-406C-A688-0D84C4E12BE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1518,4 +1486,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>